<commit_message>
Revert "[update of publications_3]"
This reverts commit 846063ee0363e8fccdf315963827c279c2b79e76.
</commit_message>
<xml_diff>
--- a/markdown_generator/publications_cesarbartolo.xlsx
+++ b/markdown_generator/publications_cesarbartolo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasec\Box\PhD DAVIS\Brandind Research\Personal Webpage_Cesar\cesarbartolo.github.io\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160C415D-A5D3-42AB-9C85-73F39C69C539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81EC227-0D32-49CC-BC40-9DC0ACAB11A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -508,8 +508,6 @@
     <col min="1" max="1" width="18.08984375" customWidth="1"/>
     <col min="2" max="2" width="17.26953125" customWidth="1"/>
     <col min="3" max="3" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="94.86328125" customWidth="1"/>
-    <col min="6" max="6" width="47.453125" customWidth="1"/>
     <col min="7" max="7" width="67.40625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>